<commit_message>
#40 create version 0.1.0
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6D0538-5A27-40A1-8B7A-537EDFCA51EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462672F1-E781-479A-8214-6562B5C4F418}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,8 @@
 Some graphics with static data are uploaded</t>
   </si>
   <si>
-    <t>Nearly same
-content as Cakedefi-Review
-uploaded</t>
+    <t>Nearly all evaluations from Cakedefi-Review.com integrated
+Adaptions made for responsive layout, especially sidebar</t>
   </si>
 </sst>
 </file>
@@ -380,7 +379,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44282</v>
       </c>

</xml_diff>

<commit_message>
changelog for next testversion
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462672F1-E781-479A-8214-6562B5C4F418}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3819D017-4B94-4167-8352-549B80492BF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,14 @@
   <si>
     <t>Nearly all evaluations from Cakedefi-Review.com integrated
 Adaptions made for responsive layout, especially sidebar</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>All graphics from Cakedefi-Review.com integrated
+Scripts are running on server and capture needed data
+First bugs are found and fixed</t>
   </si>
 </sst>
 </file>
@@ -376,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +430,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit changelog for new test release
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172A1036-80F8-4712-BE39-A466A7BC7B05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4471EDC2-D294-41F8-A194-9F43F470E48E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,12 @@
     <t>All graphics from Cakedefi-Review.com integrated
 Scripts are running on server and capture needed data
 First bugs are found and fixed</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>Next testversion with all content and fixed bugs</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +447,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44293</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changelog for 1st official version
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4471EDC2-D294-41F8-A194-9F43F470E48E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C55B52-E4C9-474E-84EE-84854B8E7645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Next testversion with all content and fixed bugs</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>First official release of DefiChain-Analytics</t>
   </si>
 </sst>
 </file>
@@ -390,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +464,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update changelog for new server version
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C55B52-E4C9-474E-84EE-84854B8E7645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B75CCDC-3E6B-4E78-829B-5D05201EC3E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,14 @@
   </si>
   <si>
     <t>First official release of DefiChain-Analytics</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>Two small bugfixes:
+- Selection in dropdown menu cannot be deleted
+- RAM issue, because of double entry in token data</t>
   </si>
 </sst>
 </file>
@@ -396,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +483,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44296</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog for version 1.1.0
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B75CCDC-3E6B-4E78-829B-5D05201EC3E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25915A69-022C-466D-8B0D-0DF136712991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8145" yWindow="3405" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +76,20 @@
     <t>Two small bugfixes:
 - Selection in dropdown menu cannot be deleted
 - RAM issue, because of double entry in token data</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>New feature:
+- masternode evaluation added
+Improvements:
+- adaptions for better mobile representation
+- DFI collateral for ERC20-token added to overview page
+- Mouse-over functionality extended to menu items
+- bottom margin for sidebar increased, that mouse over link is not hiding menu entry
+- uniform header display and removing of some figure titels (not needed ones)
+- DAA menu item renamed to "Daily active addresses"</t>
   </si>
 </sst>
 </file>
@@ -404,17 +418,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C13:C15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.7109375" customWidth="1"/>
+    <col min="3" max="3" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,6 +506,17 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44303</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adapt changelog for version 1.1.1
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25915A69-022C-466D-8B0D-0DF136712991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438D960A-D5A9-447C-8C4F-3EA5719F404E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8145" yWindow="3405" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8490" yWindow="3750" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,14 @@
 - bottom margin for sidebar increased, that mouse over link is not hiding menu entry
 - uniform header display and removing of some figure titels (not needed ones)
 - DAA menu item renamed to "Daily active addresses"</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>Improvements:
+- renaming from "active Masternodes" to "enabled Masternodes"
+- make figure height reponsive for better viewing on mobile devices</t>
   </si>
 </sst>
 </file>
@@ -418,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +527,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44304</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog to version 1.1.2
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438D960A-D5A9-447C-8C4F-3EA5719F404E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1716D0-CE2E-4AF1-B061-2992C1EC13F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="3750" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8835" yWindow="4095" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,13 @@
     <t>Improvements:
 - renaming from "active Masternodes" to "enabled Masternodes"
 - make figure height reponsive for better viewing on mobile devices</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>Improvements:
+- burned DFI added to overview</t>
   </si>
 </sst>
 </file>
@@ -426,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +545,17 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog for new version
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1716D0-CE2E-4AF1-B061-2992C1EC13F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8103277B-B6F3-4704-A3BC-842E4621D020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="4095" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="4440" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,13 @@
   <si>
     <t>Improvements:
 - burned DFI added to overview</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>Improvements:
+- after successful voting of DFIP #8 the LM-countdown is no longer needed and removed</t>
   </si>
 </sst>
 </file>
@@ -433,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +563,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44310</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog for version 1.3.0
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBF6E68-E769-46AC-A422-981E2C4246E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D2D37F-DF22-410E-BC95-F93217683FC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13095" yWindow="1275" windowWidth="21600" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -127,6 +127,23 @@
 - special DefiChain addresses now mention on explanation side of the overview
 Bugs:
 - Not working arrows in textfield of Coins addresses evaluation removed</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>New feature:
+- Evaluation of DefiChain-Promo
+- Evaluation of DefiChain marketcap
+- Donation page added
+Improvements:
+- Rework coins graphic
+- Rework address graphic
+- Show also coingecko 24hr trading volume on DEX trading volume evaluation
+- Make DefiChain-Analytics Logo as a Link to main page
+Bugs:
+- not working time selection in coins graphic
+- range selector in masternode has no active button after loading</t>
   </si>
 </sst>
 </file>
@@ -455,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +617,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update changelof for hotfix 1.3.1
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D2D37F-DF22-410E-BC95-F93217683FC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D883F47-B782-4CCD-8372-1B34D966EEB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="3660" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -144,6 +144,16 @@
 Bugs:
 - not working time selection in coins graphic
 - range selector in masternode has no active button after loading</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>Improvements:
+- Remove some print commands to reduce log-file entries
+Bugs:
+- fix Market cap graph not updated
+- remove Copy button of donation address</t>
   </si>
 </sst>
 </file>
@@ -472,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +638,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog to version 1.3.2
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D883F47-B782-4CCD-8372-1B34D966EEB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76361412-288F-4335-9EB3-C08B0BB23BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="3660" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6855" yWindow="825" windowWidth="28800" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -154,6 +154,15 @@
 Bugs:
 - fix Market cap graph not updated
 - remove Copy button of donation address</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>Improvements:
+- Change line style of absolute prices on coinprice evaluation
+- Add MyDefichain as another category to masternode evaluation
+- Reduction digits of hover label on DefiChain Promo evaluation</t>
   </si>
 </sst>
 </file>
@@ -482,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,6 +658,17 @@
         <v>28</v>
       </c>
     </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog for 1.4.0
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76361412-288F-4335-9EB3-C08B0BB23BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728675F8-0D2B-4899-8E52-3C59DF384F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6855" yWindow="825" windowWidth="28800" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -163,6 +163,17 @@
 - Change line style of absolute prices on coinprice evaluation
 - Add MyDefichain as another category to masternode evaluation
 - Reduction digits of hover label on DefiChain Promo evaluation</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
+  </si>
+  <si>
+    <t>New feature:
+- Evaluation of DefiChain-Analytics Visits
+- Evaluation of Masternode-Monitor
+Improvements:
+- Add relative change of Twitter Follower
+- Add range selector to Liquidity-Token Graph</t>
   </si>
 </sst>
 </file>
@@ -491,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,6 +680,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog for 1.4.1
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728675F8-0D2B-4899-8E52-3C59DF384F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF59907E-7ECE-4915-B6CD-196D00168EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3150" yWindow="3225" windowWidth="28800" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,14 @@
 Improvements:
 - Add relative change of Twitter Follower
 - Add range selector to Liquidity-Token Graph</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>Bugs:
+- Visualization of coins graphic was not correct (not sorted along date)
+- Tracking of all burned DFI (manual, fees and unused block rewards)</t>
   </si>
 </sst>
 </file>
@@ -502,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +699,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44353</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog for 1.4.2
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF59907E-7ECE-4915-B6CD-196D00168EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD384AE0-E70F-4EDA-822E-83516B1DA37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="3225" windowWidth="28800" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="3570" windowWidth="28800" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -182,6 +182,15 @@
     <t>Bugs:
 - Visualization of coins graphic was not correct (not sorted along date)
 - Tracking of all burned DFI (manual, fees and unused block rewards)</t>
+  </si>
+  <si>
+    <t>1.4.2</t>
+  </si>
+  <si>
+    <t>Improvements:
+- Change scaling block time
+Bugs:
+- Coins graphic with strange behavior =&gt; double entries</t>
   </si>
 </sst>
 </file>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C26" sqref="C22:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +719,17 @@
         <v>34</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44359</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog to 1.5.0
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD384AE0-E70F-4EDA-822E-83516B1DA37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A39DD9E-9583-4D1D-A971-6919062B4200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="3570" windowWidth="28800" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -191,6 +191,16 @@
 - Change scaling block time
 Bugs:
 - Coins graphic with strange behavior =&gt; double entries</t>
+  </si>
+  <si>
+    <t>1.5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New feature:
+- Evaluation of minted blocks per day
+- Evaluation of DEX price stability
+Improvements:
+- Evaluation of DefiChain-Promo user numbers </t>
   </si>
 </sst>
 </file>
@@ -519,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C22:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,6 +740,17 @@
         <v>36</v>
       </c>
     </row>
+    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog to 1.5.1
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A39DD9E-9583-4D1D-A971-6919062B4200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA977EB1-F476-49D1-9909-D0AD7FE15F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6855" yWindow="4110" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,13 @@
 - Evaluation of DEX price stability
 Improvements:
 - Evaluation of DefiChain-Promo user numbers </t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>Improvements:
+- show circ supply, total cupply, market cap and corresponding rank also for missing DFI token. NaN-entry handled as Zero and user gets a hint of not correct values.</t>
   </si>
 </sst>
 </file>
@@ -529,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +758,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adapt changelog to 1.5.2
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA977EB1-F476-49D1-9909-D0AD7FE15F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7E98E9-B426-4448-AFAE-7407A186AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6855" yWindow="4110" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7890" yWindow="5145" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -208,6 +208,13 @@
   <si>
     <t>Improvements:
 - show circ supply, total cupply, market cap and corresponding rank also for missing DFI token. NaN-entry handled as Zero and user gets a hint of not correct values.</t>
+  </si>
+  <si>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>Bugs:
+- Wrong representation of links (color is standard blue instead of pink) fixed</t>
   </si>
 </sst>
 </file>
@@ -536,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +776,17 @@
         <v>40</v>
       </c>
     </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#141 update changelog, correct TokenData.csv
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7E98E9-B426-4448-AFAE-7407A186AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366BE875-B19D-48C1-B800-BF224F80DEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="5145" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,21 @@
   <si>
     <t>Bugs:
 - Wrong representation of links (color is standard blue instead of pink) fixed</t>
+  </si>
+  <si>
+    <t>1.5.3</t>
+  </si>
+  <si>
+    <t>Update graphics for new USDC-pool. The following evaluations were changed
+- Overview
+- Coins
+- Coinprices
+- Volume
+- Price stability
+- TVL
+- Liquidity Token
+- Fees
+- Cryptos-DAT</t>
   </si>
 </sst>
 </file>
@@ -543,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,6 +802,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="22" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44415</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#220 adapt circulating supply
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE95A6F-2B18-48CB-A12A-2EB52B30EAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40533B7B-C7B7-405D-84C5-9B2C5DFF5CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="3195" windowWidth="27285" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="4500" windowWidth="28800" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -405,6 +413,13 @@
 - Change scaling of dUSD price graph
 - Rework of DFX evaluation
 - New calculation of DFI Token </t>
+  </si>
+  <si>
+    <t>2.5.1</t>
+  </si>
+  <si>
+    <t>Improvement:
+- Adapt circulating supply in Overview and Coins evaluation</t>
   </si>
 </sst>
 </file>
@@ -733,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C44"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,6 +1179,17 @@
         <v>76</v>
       </c>
     </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>44648</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#221 add dTokens to APR view
</commit_message>
<xml_diff>
--- a/data/changelogHistory.xlsx
+++ b/data/changelogHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Daten\Kryptowährung\Cake\DefiChainAnalytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8D5B7E-C2FA-4094-BC43-0A90BD57AFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCD0241-58F7-48E1-B545-01EA34476FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   </si>
   <si>
     <t>Improvement:
-- Add new dTokens to the evaluations: Liquidity Token, dToken prices, Number dToken</t>
+- Add new dTokens to the evaluations: Liquidity Token, dToken prices, Number dToken, premium dToken, APR rates</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1197,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44653</v>
       </c>

</xml_diff>